<commit_message>
- fix delete history command
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgi\Documents\GitHub\scala_weather_bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FMI\3 year\6 term\Scala\hw\final_project\final-project-team-scala_weather_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBE64ED-333B-4D48-A9E5-3E9D02C94009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AA7F26-A33E-4694-9C48-90454CCB0C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="current" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>unidentified</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Command</t>
   </si>
   <si>
-    <t>{"location":{"name":"Sofia","region":"Grad Sofiya","country":"Bulgaria","lat":42.68,"lon":23.32,"tz_id":"Europe/Sofia","localtime_epoch":1655734471,"localtime":"2022-06-20 17:14"},"current":{"last_updated_epoch":1655730000,"last_updated":"2022-06-20 16:00","temp_c":26.0,"temp_f":78.8,"is_day":1,"condition":{"text":"Sunny","icon":"//cdn.weatherapi.com/weather/64x64/day/113.png","code":1000},"wind_mph":4.3,"wind_kph":6.8,"wind_degree":60,"wind_dir":"ENE","pressure_mb":1014.0,"pressure_in":29.94,"precip_mm":0.0,"precip_in":0.0,"humidity":39,"cloud":0,"feelslike_c":25.5,"feelslike_f":77.8,"vis_km":10.0,"vis_miles":6.0,"uv":7.0,"gust_mph":3.8,"gust_kph":6.1}}</t>
-  </si>
-  <si>
-    <t>{"location":{"name":"Sofia","region":"Grad Sofiya","country":"Bulgaria","lat":42.68,"lon":23.32,"tz_id":"Europe/Sofia","localtime_epoch":1655735169,"localtime":"2022-06-20 17:26"},"current":{"last_updated_epoch":1655734500,"last_updated":"2022-06-20 17:15","temp_c":26.0,"temp_f":78.8,"is_day":1,"condition":{"text":"Sunny","icon":"//cdn.weatherapi.com/weather/64x64/day/113.png","code":1000},"wind_mph":3.8,"wind_kph":6.1,"wind_degree":280,"wind_dir":"W","pressure_mb":1013.0,"pressure_in":29.91,"precip_mm":0.0,"precip_in":0.0,"humidity":39,"cloud":0,"feelslike_c":25.5,"feelslike_f":77.8,"vis_km":10.0,"vis_miles":6.0,"uv":7.0,"gust_mph":3.8,"gust_kph":6.1}}</t>
-  </si>
-  <si>
     <t>List(Mon, 20 Jun 2022 14:32:22 GMT)</t>
   </si>
   <si>
@@ -57,16 +51,22 @@
     <t>List(Mon, 20 Jun 2022 14:50:51 GMT)</t>
   </si>
   <si>
-    <t>{"football":[{"stadium":"Fc Rapid Bucuresti","country":"Romania","region":"","tournament":"UEFA Nations League","start":"2022-06-14 19:45","match":"Romania vs Montenegro"},{"stadium":"Inter Turku , Fc Tps","country":"Finland","region":"","tournament":"Finnish Veikkausliga","start":"2022-06-22 16:00","match":"FC Inter Turku vs FC Lahti"},{"stadium":"Drogheda United","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"Drogheda vs Sligo Rovers"},{"stadium":"Shelbourne Fc","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"Shelbourne vs Dundalk"},{"stadium":"Ucd","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"U.C.D vs Derry City"},{"stadium":"Cork City Fc","country":"Ireland","region":"","tournament":"League of Ireland First Division","start":"2022-06-24 19:45","match":"Cork City vs Cobh Ramblers"},{"stadium":"Waterford United Fc","country":"Ireland","region":"","tournament":"League of Ireland First Division","start":"2022-06-24 19:45","match":"Waterford United vs Bray Wanderers"},{"stadium":"Finn Harps","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 20:00","match":"Finn Harps vs St Patricks Athletic"},{"stadium":"Shamrock Rovers(A)","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 20:00","match":"Shamrock Rovers vs Bohemians"},{"stadium":"Cincinnati Kings","country":"United States of America","region":"","tournament":"American MLS League","start":"2022-06-25 00:30","match":"FC Cincinnati vs Orlando City SC"}],"cricket":[{"stadium":"Sir Vivian Richards Stadium, North Sound, Antigua","country":"West Indies","region":"","tournament":"West Indies vs Bangladesh Test Series 2022","start":"2022-06-16 15:00","match":"West Indies vs Bangladesh"},{"stadium":"R.Premadasa Stadium, Khettarama, Colombo","country":"Sri Lanka","region":"","tournament":"Sri Lanka vs Australia ODI Series 2022","start":"2022-06-21 10:00","match":"Sri Lanka vs Australia"}],"golf":[{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:35","match":"Lucas Herbert, Chan Kim"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:45","match":"Ryan Moore, Adam Scott"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:55","match":"Aaron Rai, Adam Schenk"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 13:05","match":"Kramer Hickok, David Lingmerth"}]}</t>
-  </si>
-  <si>
     <t>football</t>
   </si>
   <si>
     <t>List(Tue, 21 Jun 2022 08:14:39 GMT)</t>
   </si>
   <si>
-    <t>{"football":[{"stadium":"Fc Rapid Bucuresti","country":"Romania","region":"","tournament":"UEFA Nations League","start":"2022-06-14 19:45","match":"Romania vs Montenegro"},{"stadium":"Inter Turku , Fc Tps","country":"Finland","region":"","tournament":"Finnish Veikkausliga","start":"2022-06-22 16:00","match":"FC Inter Turku vs FC Lahti"},{"stadium":"Drogheda United","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"Drogheda vs Sligo Rovers"},{"stadium":"Shelbourne Fc","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"Shelbourne vs Dundalk"},{"stadium":"Ucd","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"U.C.D vs Derry City"},{"stadium":"Cork City Fc","country":"Ireland","region":"","tournament":"League of Ireland First Division","start":"2022-06-24 19:45","match":"Cork City vs Cobh Ramblers"},{"stadium":"Waterford United Fc","country":"Ireland","region":"","tournament":"League of Ireland First Division","start":"2022-06-24 19:45","match":"Waterford United vs Bray Wanderers"},{"stadium":"Finn Harps","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 20:00","match":"Finn Harps vs St Patricks Athletic"},{"stadium":"Shamrock Rovers(A)","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 20:00","match":"Shamrock Rovers vs Bohemians"},{"stadium":"Cincinnati Kings","country":"United States of America","region":"","tournament":"American MLS League","start":"2022-06-25 00:30","match":"FC Cincinnati vs Orlando City SC"}],"cricket":[{"stadium":"R.Premadasa Stadium, Khettarama, Colombo","country":"Sri Lanka","region":"","tournament":"Sri Lanka vs Australia ODI Series 2022","start":"2022-06-21 10:00","match":"Sri Lanka vs Australia"}],"golf":[{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:35","match":"Lucas Herbert, Chan Kim"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:45","match":"Ryan Moore, Adam Scott"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:55","match":"Aaron Rai, Adam Schenk"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 13:05","match":"Kramer Hickok, David Lingmerth"}]}</t>
+    <t>{"location":{"name":"Plovdiv","region":"Grad Plovdiv","country":"Bulgaria","lat":42.68,"lon":23.32,"tz_id":"Europe/Sofia","localtime_epoch":1655735169,"localtime":"2022-06-20 17:26"},"current":{"last_updated_epoch":1655734500,"last_updated":"2022-06-20 17:15","temp_c":26.0,"temp_f":78.8,"is_day":1,"condition":{"text":"Sunny","icon":"//cdn.weatherapi.com/weather/64x64/day/113.png","code":1000},"wind_mph":3.8,"wind_kph":6.1,"wind_degree":280,"wind_dir":"W","pressure_mb":1013.0,"pressure_in":29.91,"precip_mm":0.0,"precip_in":0.0,"humidity":39,"cloud":0,"feelslike_c":25.5,"feelslike_f":77.8,"vis_km":10.0,"vis_miles":6.0,"uv":7.0,"gust_mph":3.8,"gust_kph":6.1}}</t>
+  </si>
+  <si>
+    <t>{"location":{"name":"Asenovgrad","region":" Asenovgrad","country":"Bulgaria","lat":42.68,"lon":23.32,"tz_id":"Europe/Sofia","localtime_epoch":1655734471,"localtime":"2022-06-20 17:14"},"current":{"last_updated_epoch":1655730000,"last_updated":"2022-06-20 16:00","temp_c":26.0,"temp_f":78.8,"is_day":1,"condition":{"text":"Sunny","icon":"//cdn.weatherapi.com/weather/64x64/day/113.png","code":1000},"wind_mph":4.3,"wind_kph":6.8,"wind_degree":60,"wind_dir":"ENE","pressure_mb":1014.0,"pressure_in":29.94,"precip_mm":0.0,"precip_in":0.0,"humidity":39,"cloud":0,"feelslike_c":25.5,"feelslike_f":77.8,"vis_km":10.0,"vis_miles":6.0,"uv":7.0,"gust_mph":3.8,"gust_kph":6.1}}</t>
+  </si>
+  <si>
+    <t>{"football":[{"stadium":"Fc Rapid Bucuresti","country":"Romania","region":"","tournament":"UEFA Nations League","start":"2022-06-14 19:45","match":"Romania vs Montenegro"},{"stadium":"Inter Turku , Fc Tps","country":"Finland","region":"","tournament":"Finnish Veikkausliga","start":"2022-06-22 16:00","match":"FC Inter Turku vs FC Lahti"},{"stadium":"Drogheda United","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"Drogheda vs Sligo Rovers"},{"stadium":"Shelbourne Fc","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"Shelbourne vs Dundalk"},{"stadium":"Ucd","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"U.C.D vs Derry City"},{"stadium":"Cork City Fc","country":"Ireland","region":"","tournament":"League of Ireland First Division","start":"2022-06-24 19:45","match":"Cork City vs Cobh Ramblers"},{"stadium":"Waterford United Fc","country":"Ireland","region":"","tournament":"League of Ireland First Division","start":"2022-06-24 19:45","match":"Waterford United vs Bray Wanderers"},{"stadium":"Finn Harps","country":"Bulgaria","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 20:00","match":"Finn Harps vs St Patricks Athletic"},{"stadium":"Shamrock Rovers(A)","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 20:00","match":"Shamrock Rovers vs Bohemians"},{"stadium":"Cincinnati Kings","country":"United States of America","region":"","tournament":"American MLS League","start":"2022-06-25 00:30","match":"FC Cincinnati vs Orlando City SC"}],"cricket":[{"stadium":"Sir Vivian Richards Stadium, North Sound, Antigua","country":"West Indies","region":"","tournament":"West Indies vs Bangladesh Test Series 2022","start":"2022-06-16 15:00","match":"West Indies vs Bangladesh"},{"stadium":"R.Premadasa Stadium, Khettarama, Colombo","country":"Sri Lanka","region":"","tournament":"Sri Lanka vs Australia ODI Series 2022","start":"2022-06-21 10:00","match":"Sri Lanka vs Australia"}],"golf":[{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:35","match":"Lucas Herbert, Chan Kim"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:45","match":"Ryan Moore, Adam Scott"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:55","match":"Aaron Rai, Adam Schenk"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 13:05","match":"Kramer Hickok, David Lingmerth"}]}</t>
+  </si>
+  <si>
+    <t>{"football":[{"stadium":"Fc Rapid Bucuresti","country":"Romania","region":"","tournament":"UEFA Nations League","start":"2022-06-14 19:45","match":"Romania vs Montenegro"},{"stadium":"Inter Turku , Fc Tps","country":"Finland","region":"","tournament":"Finnish Veikkausliga","start":"2022-06-22 16:00","match":"FC Inter Turku vs FC Lahti"},{"stadium":"Drogheda United","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"Drogheda vs Sligo Rovers"},{"stadium":"Shelbourne Fc","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"Shelbourne vs Dundalk"},{"stadium":"Ucd","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 19:45","match":"U.C.D vs Derry City"},{"stadium":"Cork City Fc","country":"Ireland","region":"","tournament":"League of Ireland First Division","start":"2022-06-24 19:45","match":"Cork City vs Cobh Ramblers"},{"stadium":"Waterford United Fc","country":"Ireland","region":"","tournament":"League of Ireland First Division","start":"2022-06-24 19:45","match":"Waterford United vs Bray Wanderers"},{"stadium":"Finn Harps","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 20:00","match":"Finn Harps vs St Patricks Athletic"},{"stadium":"Shamrock Rovers(A)","country":"Ireland","region":"","tournament":"League of Ireland Premier Division","start":"2022-06-24 20:00","match":"Shamrock Rovers vs Bohemians"},{"stadium":"Cincinnati Kings","country":"Sofia","region":"","tournament":"American MLS League","start":"2022-06-25 00:30","match":"FC Cincinnati vs Orlando City SC"}],"cricket":[{"stadium":"R.Premadasa Stadium, Khettarama, Colombo","country":"Sri Lanka","region":"","tournament":"Sri Lanka vs Australia ODI Series 2022","start":"2022-06-21 10:00","match":"Sri Lanka vs Australia"}],"golf":[{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:35","match":"Lucas Herbert, Chan Kim"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:45","match":"Ryan Moore, Adam Scott"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 12:55","match":"Aaron Rai, Adam Schenk"},{"stadium":"Muirfield Village Gc","country":"United States of America","region":"","tournament":"the Memorial Tournament presented by Workday Round 3","start":"2022-06-04 13:05","match":"Kramer Hickok, David Lingmerth"}]}</t>
   </si>
 </sst>
 </file>
@@ -107,7 +107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -123,9 +123,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,7 +163,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -269,7 +269,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0A0B30-3EAF-4719-A95A-4E08631A2B9C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,62 +441,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -504,54 +448,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D73B42-6634-45A3-BB7E-9F8B4BA3DC55}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105157DD-FA33-4138-93E8-DDDF57638882}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105157DD-FA33-4138-93E8-DDDF57638882}">
+  <dimension ref="A2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>